<commit_message>
finish manage image folder
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudyDocuments\Capstone\SourceCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudyDocuments\Capstone\capstone-project-employee\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA096A-9890-4042-923E-02DB524F52FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EB554E-C447-4E19-B5EF-3C1E87116571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,14 +58,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Brand</t>
-  </si>
-  <si>
     <t>Loại hàng</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>Số lượng</t>
   </si>
   <si>
-    <t>Giá thật</t>
-  </si>
-  <si>
-    <t>Giá thuê</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -96,27 +87,6 @@
     <t>Tình Trạng</t>
   </si>
   <si>
-    <t>Cho thuê</t>
-  </si>
-  <si>
-    <t>File ảnh chính</t>
-  </si>
-  <si>
-    <t>File ảnh 1</t>
-  </si>
-  <si>
-    <t>File ảnh 2</t>
-  </si>
-  <si>
-    <t>File ảnh 3</t>
-  </si>
-  <si>
-    <t>File ảnh 4</t>
-  </si>
-  <si>
-    <t>File ảnh 5</t>
-  </si>
-  <si>
     <t>Victor</t>
   </si>
   <si>
@@ -217,6 +187,30 @@
   </si>
   <si>
     <t>Golf</t>
+  </si>
+  <si>
+    <t>Thương hiệu</t>
+  </si>
+  <si>
+    <t>Giá bán</t>
+  </si>
+  <si>
+    <t>Link ảnh chính</t>
+  </si>
+  <si>
+    <t>Link ảnh 1</t>
+  </si>
+  <si>
+    <t>Link ảnh 2</t>
+  </si>
+  <si>
+    <t>Link ảnh 3</t>
+  </si>
+  <si>
+    <t>Link ảnh 4</t>
+  </si>
+  <si>
+    <t>Link ảnh 5</t>
   </si>
 </sst>
 </file>
@@ -833,112 +827,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD111"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="16" width="10.5546875" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" customWidth="1"/>
-    <col min="19" max="19" width="9.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="15" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:21">
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="3" spans="1:23">
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
       <c r="L3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="Q3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="R3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="S3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="T3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="U3" t="s">
-        <v>16</v>
-      </c>
-      <c r="V3" t="s">
-        <v>17</v>
-      </c>
-      <c r="W3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{F8469D2E-41EC-4F4C-9787-74C755072773}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -984,10 +968,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -995,7 +979,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1003,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1011,7 +995,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1019,7 +1003,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1027,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1038,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1065,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1073,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1081,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1089,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1097,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1105,7 +1089,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1113,7 +1097,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1121,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1129,7 +1113,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1137,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1164,10 +1148,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1175,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1183,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1191,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1199,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1207,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1215,7 +1199,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1223,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1231,7 +1215,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1239,7 +1223,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1247,7 +1231,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1255,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>